<commit_message>
SSDM-13256: Added missing columns for vocabulary type.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-vocabulary.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
   </si>
@@ -31,10 +31,28 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Registrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANTIBODY.DETECTION</t>
   </si>
   <si>
     <t xml:space="preserve">Protein detection system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-10 17:23:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-11 17:23:44</t>
   </si>
   <si>
     <t xml:space="preserve">Label</t>
@@ -62,8 +80,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -144,7 +163,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,6 +173,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,33 +197,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="17.99"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,7 +252,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -216,24 +260,24 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>